<commit_message>
feat: tratamento v3 NOVEMBRO 2022
</commit_message>
<xml_diff>
--- a/Base de Dados/Dados Tratados v3/1. OUTUBRO_2022_PRODUTIVIDADE.xlsx
+++ b/Base de Dados/Dados Tratados v3/1. OUTUBRO_2022_PRODUTIVIDADE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\GitHub\Projeto-Painel-de-BI-Dados-Agricolas\Base de Dados\Dados Tratados v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F28C60-19C2-4A07-9847-18C02B0933BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E8C579-9879-4F18-A716-E918EAF5CCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1481,7 +1481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A91FE5-B1B8-4AC0-AF52-A2F1E5238C66}">
   <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>